<commit_message>
add item and magic.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/ItemData.xlsx
+++ b/Documents/ExcelData/ItemData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -97,7 +97,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>itemID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原力之瓶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复生命值至80%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>万物皆空，万事皆允</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>magicID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>或许是某种神秘的灵气之力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skillID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火球之书</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰弹之书</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>闪电之书</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记载了火球术用法的古老书籍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记载了闪电术用法的古老书籍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记载了冰弹术用法的古老书籍</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -458,12 +522,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -471,18 +574,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="8.875" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -510,8 +614,11 @@
       <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -539,8 +646,11 @@
       <c r="I2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1100</v>
       </c>
@@ -568,8 +678,11 @@
       <c r="I3">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1101</v>
       </c>
@@ -597,8 +710,11 @@
       <c r="I4">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1200</v>
       </c>
@@ -626,8 +742,11 @@
       <c r="I5">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1201</v>
       </c>
@@ -655,8 +774,11 @@
       <c r="I6">
         <v>107</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1300</v>
       </c>
@@ -684,8 +806,11 @@
       <c r="I7">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1301</v>
       </c>
@@ -713,8 +838,11 @@
       <c r="I8">
         <v>108</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1400</v>
       </c>
@@ -742,8 +870,11 @@
       <c r="I9">
         <v>104</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1401</v>
       </c>
@@ -771,8 +902,11 @@
       <c r="I10">
         <v>109</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1500</v>
       </c>
@@ -800,8 +934,11 @@
       <c r="I11">
         <v>105</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1501</v>
       </c>
@@ -828,6 +965,9 @@
       </c>
       <c r="I12">
         <v>110</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -839,25 +979,146 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:H1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="8" max="8" width="26.375" customWidth="1"/>
+    <col min="9" max="9" width="8.875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>2000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <v>80</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>201</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>90</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>202</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>80</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <v>110</v>
+      </c>
+      <c r="G5">
+        <v>203</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a draft of BuffData.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/ItemData.xlsx
+++ b/Documents/ExcelData/ItemData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -981,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
data correction and counter formula.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/ItemData.xlsx
+++ b/Documents/ExcelData/ItemData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
   <si>
     <t>name</t>
   </si>
@@ -122,10 +122,6 @@
   </si>
   <si>
     <t>武器暴击率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>武器打断值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -241,18 +237,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>速度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>命中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>暴击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>技能ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -373,7 +357,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>法术打断值</t>
+    <t>武器击退值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法术击退值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法术命中率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法术暴击率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法术速度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -783,7 +783,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -793,18 +793,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
@@ -815,13 +815,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -858,7 +858,7 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I14"/>
+      <selection activeCell="M1" sqref="M1:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -866,9 +866,10 @@
     <col min="3" max="3" width="39.375" customWidth="1"/>
     <col min="4" max="4" width="11.75" customWidth="1"/>
     <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="10.125" customWidth="1"/>
-    <col min="7" max="7" width="10.25" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11.625" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="10.5" customWidth="1"/>
     <col min="12" max="12" width="9.75" customWidth="1"/>
@@ -884,7 +885,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>20</v>
@@ -902,27 +903,27 @@
         <v>24</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -946,7 +947,7 @@
         <v>7</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>1</v>
@@ -958,54 +959,54 @@
         <v>5</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1060,7 +1061,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -1097,10 +1098,10 @@
         <v>1200</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -1137,10 +1138,10 @@
         <v>1300</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="1">
         <v>9</v>
@@ -1180,7 +1181,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1">
         <v>8</v>
@@ -1217,10 +1218,10 @@
         <v>1500</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D9" s="1">
         <v>12</v>
@@ -1257,10 +1258,10 @@
         <v>1600</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1">
         <v>16</v>
@@ -1297,10 +1298,10 @@
         <v>1700</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1">
         <v>11</v>
@@ -1337,10 +1338,10 @@
         <v>1800</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1">
         <v>16</v>
@@ -1377,10 +1378,10 @@
         <v>3001</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1417,10 +1418,10 @@
         <v>3002</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D14" s="1">
         <v>25</v>
@@ -1863,29 +1864,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="10.125" customWidth="1"/>
     <col min="3" max="3" width="34.625" customWidth="1"/>
+    <col min="6" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="7" width="12.125" customWidth="1"/>
+    <col min="8" max="8" width="11.375" customWidth="1"/>
     <col min="9" max="9" width="11.75" customWidth="1"/>
     <col min="11" max="11" width="8.875" customWidth="1"/>
+    <col min="12" max="12" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="C1" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>20</v>
@@ -1893,25 +1898,31 @@
       <c r="E1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="8" t="s">
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="J1" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
@@ -1926,54 +1937,66 @@
         <v>23</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="I2" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+        <v>60</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A4" s="8">
         <v>2000</v>
       </c>
@@ -2004,16 +2027,22 @@
       <c r="J4" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2001</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -2022,13 +2051,13 @@
         <v>25</v>
       </c>
       <c r="F5">
+        <v>80</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>60</v>
-      </c>
-      <c r="G5">
-        <v>80</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -2037,15 +2066,15 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2002</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -2057,10 +2086,10 @@
         <v>100</v>
       </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>100</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -2069,15 +2098,15 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2003</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -2086,13 +2115,13 @@
         <v>20</v>
       </c>
       <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>80</v>
-      </c>
-      <c r="G7">
-        <v>90</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -2101,15 +2130,15 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>4001</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2121,10 +2150,10 @@
         <v>100</v>
       </c>
       <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>100</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -2133,15 +2162,15 @@
         <v>4001</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>4002</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D9">
         <v>200</v>
@@ -2150,13 +2179,13 @@
         <v>255</v>
       </c>
       <c r="F9">
+        <v>80</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>60</v>
-      </c>
-      <c r="G9">
-        <v>80</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -2165,15 +2194,15 @@
         <v>4002</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>4003</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D10">
         <v>190</v>
@@ -2185,10 +2214,10 @@
         <v>100</v>
       </c>
       <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>100</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -2197,15 +2226,15 @@
         <v>4003</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>4004</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D11">
         <v>220</v>
@@ -2214,13 +2243,13 @@
         <v>250</v>
       </c>
       <c r="F11">
+        <v>90</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>80</v>
-      </c>
-      <c r="G11">
-        <v>90</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2229,13 +2258,13 @@
         <v>4004</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="I14" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move cost from skillData to ItemData.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/ItemData.xlsx
+++ b/Documents/ExcelData/ItemData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChineseRoguelikeGame\Documents\ExcelData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="22935" windowHeight="9825" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22935" windowHeight="9825" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="450">
   <si>
     <t>物品ID</t>
   </si>
@@ -83,7 +88,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>+1</t>
     </r>
@@ -106,7 +111,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>+2</t>
     </r>
@@ -129,7 +134,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>+3</t>
     </r>
@@ -152,7 +157,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>+4</t>
     </r>
@@ -175,7 +180,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>+5</t>
     </r>
@@ -198,7 +203,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>LV.2</t>
     </r>
@@ -230,7 +235,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>LV.3</t>
     </r>
@@ -262,7 +267,7 @@
         <sz val="10.5"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>LV.4</t>
     </r>
@@ -1479,7 +1484,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>[</t>
     </r>
@@ -1497,7 +1502,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>]</t>
     </r>
@@ -1565,18 +1570,38 @@
   <si>
     <t>“被幽灵注视着，不自觉地全身酥麻，绵软无力”</t>
   </si>
+  <si>
+    <t>法术消耗</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LOAT</t>
+    </r>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="31">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1630,154 +1655,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1795,10 +1676,32 @@
       <sz val="10.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1811,194 +1714,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2006,253 +1723,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2286,7 +1761,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2330,58 +1805,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2428,7 +1869,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2463,7 +1904,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2671,15 +2112,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="19.75" customWidth="1"/>
     <col min="3" max="3" width="21.625" customWidth="1"/>
@@ -2762,7 +2202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" ht="14.25" spans="1:3">
+    <row r="8" spans="1:3" ht="15">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2773,7 +2213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" ht="14.25" spans="1:3">
+    <row r="9" spans="1:3" ht="15">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2784,7 +2224,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" ht="14.25" spans="1:3">
+    <row r="10" spans="1:3" ht="15">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2795,7 +2235,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" ht="14.25" spans="1:3">
+    <row r="11" spans="1:3" ht="15">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2806,7 +2246,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" ht="14.25" spans="1:3">
+    <row r="12" spans="1:3" ht="15">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2817,7 +2257,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" ht="14.25" spans="1:3">
+    <row r="13" spans="1:3" ht="15">
       <c r="A13">
         <v>101</v>
       </c>
@@ -2828,7 +2268,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" ht="14.25" spans="1:3">
+    <row r="14" spans="1:3" ht="15">
       <c r="A14">
         <v>102</v>
       </c>
@@ -2839,7 +2279,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" ht="14.25" spans="1:3">
+    <row r="15" spans="1:3" ht="15">
       <c r="A15">
         <v>103</v>
       </c>
@@ -2851,15 +2291,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q176"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
@@ -2939,7 +2378,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" ht="27" spans="1:17">
+    <row r="2" spans="1:17" ht="27">
       <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
@@ -3045,7 +2484,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:17">
+    <row r="4" spans="1:17" ht="15" customHeight="1">
       <c r="A4" s="19">
         <v>1000</v>
       </c>
@@ -3380,7 +2819,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" customFormat="1" spans="1:17">
+    <row r="11" spans="1:17">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
@@ -3399,7 +2838,7 @@
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
     </row>
-    <row r="12" customFormat="1" spans="1:17">
+    <row r="12" spans="1:17">
       <c r="A12" s="21">
         <v>1110</v>
       </c>
@@ -3442,7 +2881,7 @@
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
     </row>
-    <row r="13" customFormat="1" spans="1:17">
+    <row r="13" spans="1:17">
       <c r="A13" s="21" t="s">
         <v>99</v>
       </c>
@@ -3485,7 +2924,7 @@
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
     </row>
-    <row r="14" customFormat="1" spans="1:17">
+    <row r="14" spans="1:17">
       <c r="A14" s="21" t="s">
         <v>101</v>
       </c>
@@ -3528,7 +2967,7 @@
       <c r="P14" s="24"/>
       <c r="Q14" s="24"/>
     </row>
-    <row r="15" customFormat="1" spans="1:17">
+    <row r="15" spans="1:17">
       <c r="A15" s="21" t="s">
         <v>104</v>
       </c>
@@ -3571,7 +3010,7 @@
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
     </row>
-    <row r="16" customFormat="1" spans="1:17">
+    <row r="16" spans="1:17">
       <c r="A16" s="21" t="s">
         <v>107</v>
       </c>
@@ -3614,7 +3053,7 @@
       <c r="P16" s="24"/>
       <c r="Q16" s="24"/>
     </row>
-    <row r="17" customFormat="1" spans="1:17">
+    <row r="17" spans="1:17">
       <c r="A17" s="21" t="s">
         <v>111</v>
       </c>
@@ -3657,7 +3096,7 @@
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
     </row>
-    <row r="18" customFormat="1" spans="1:17">
+    <row r="18" spans="1:17">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
@@ -4051,7 +3490,7 @@
       <c r="P27" s="24"/>
       <c r="Q27" s="24"/>
     </row>
-    <row r="28" customFormat="1" spans="1:17">
+    <row r="28" spans="1:17">
       <c r="A28" s="21" t="s">
         <v>146</v>
       </c>
@@ -4100,7 +3539,7 @@
       <c r="P28" s="24"/>
       <c r="Q28" s="24"/>
     </row>
-    <row r="29" customFormat="1" spans="1:17">
+    <row r="29" spans="1:17">
       <c r="A29" s="21" t="s">
         <v>148</v>
       </c>
@@ -4149,7 +3588,7 @@
       <c r="P29" s="24"/>
       <c r="Q29" s="24"/>
     </row>
-    <row r="30" customFormat="1" spans="1:17">
+    <row r="30" spans="1:17">
       <c r="A30" s="21" t="s">
         <v>152</v>
       </c>
@@ -4198,7 +3637,7 @@
       <c r="P30" s="24"/>
       <c r="Q30" s="24"/>
     </row>
-    <row r="31" customFormat="1" spans="1:17">
+    <row r="31" spans="1:17">
       <c r="A31" s="21" t="s">
         <v>155</v>
       </c>
@@ -7695,7 +7134,7 @@
       <c r="P119" s="24"/>
       <c r="Q119" s="24"/>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:17">
       <c r="A120" s="17"/>
       <c r="B120" s="17"/>
       <c r="D120" s="17"/>
@@ -7710,7 +7149,7 @@
       <c r="M120" s="28"/>
       <c r="N120" s="28"/>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:17">
       <c r="A121" s="17"/>
       <c r="B121" s="17"/>
       <c r="D121" s="17"/>
@@ -7725,7 +7164,7 @@
       <c r="M121" s="28"/>
       <c r="N121" s="28"/>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:17">
       <c r="A122" s="17"/>
       <c r="B122" s="17"/>
       <c r="D122" s="17"/>
@@ -7740,7 +7179,7 @@
       <c r="M122" s="28"/>
       <c r="N122" s="28"/>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:17">
       <c r="A123" s="17"/>
       <c r="B123" s="26"/>
       <c r="C123" s="27"/>
@@ -7756,7 +7195,7 @@
       <c r="M123" s="28"/>
       <c r="N123" s="28"/>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:17">
       <c r="A124" s="17"/>
       <c r="B124" s="17"/>
       <c r="D124" s="17"/>
@@ -7771,7 +7210,7 @@
       <c r="M124" s="28"/>
       <c r="N124" s="28"/>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:17">
       <c r="A125" s="17"/>
       <c r="B125" s="17"/>
       <c r="D125" s="17"/>
@@ -7786,7 +7225,7 @@
       <c r="M125" s="28"/>
       <c r="N125" s="28"/>
     </row>
-    <row r="126" spans="1:14">
+    <row r="126" spans="1:17">
       <c r="A126" s="17"/>
       <c r="B126" s="17"/>
       <c r="D126" s="17"/>
@@ -7801,7 +7240,7 @@
       <c r="M126" s="28"/>
       <c r="N126" s="28"/>
     </row>
-    <row r="127" spans="1:14">
+    <row r="127" spans="1:17">
       <c r="A127" s="17"/>
       <c r="B127" s="17"/>
       <c r="D127" s="17"/>
@@ -7816,7 +7255,7 @@
       <c r="M127" s="29"/>
       <c r="N127" s="29"/>
     </row>
-    <row r="128" spans="1:14">
+    <row r="128" spans="1:17">
       <c r="A128" s="17"/>
       <c r="B128" s="17"/>
       <c r="D128" s="17"/>
@@ -7876,85 +7315,85 @@
       <c r="M131" s="29"/>
       <c r="N131" s="29"/>
     </row>
-    <row r="132" spans="10:14">
+    <row r="132" spans="1:14">
       <c r="J132" s="17"/>
       <c r="K132" s="17"/>
       <c r="L132" s="17"/>
       <c r="M132" s="29"/>
       <c r="N132" s="29"/>
     </row>
-    <row r="133" spans="10:14">
+    <row r="133" spans="1:14">
       <c r="J133" s="17"/>
       <c r="K133" s="17"/>
       <c r="L133" s="17"/>
       <c r="M133" s="29"/>
       <c r="N133" s="29"/>
     </row>
-    <row r="134" spans="10:14">
+    <row r="134" spans="1:14">
       <c r="J134" s="17"/>
       <c r="K134" s="17"/>
       <c r="L134" s="17"/>
       <c r="M134" s="29"/>
       <c r="N134" s="29"/>
     </row>
-    <row r="135" spans="10:14">
+    <row r="135" spans="1:14">
       <c r="J135" s="17"/>
       <c r="K135" s="17"/>
       <c r="L135" s="17"/>
       <c r="M135" s="29"/>
       <c r="N135" s="29"/>
     </row>
-    <row r="136" spans="10:14">
+    <row r="136" spans="1:14">
       <c r="J136" s="17"/>
       <c r="K136" s="17"/>
       <c r="L136" s="17"/>
       <c r="M136" s="29"/>
       <c r="N136" s="29"/>
     </row>
-    <row r="137" spans="10:14">
+    <row r="137" spans="1:14">
       <c r="J137" s="17"/>
       <c r="K137" s="17"/>
       <c r="L137" s="17"/>
       <c r="M137" s="29"/>
       <c r="N137" s="29"/>
     </row>
-    <row r="138" spans="10:14">
+    <row r="138" spans="1:14">
       <c r="J138" s="17"/>
       <c r="K138" s="17"/>
       <c r="L138" s="17"/>
       <c r="M138" s="29"/>
       <c r="N138" s="29"/>
     </row>
-    <row r="139" spans="10:14">
+    <row r="139" spans="1:14">
       <c r="J139" s="17"/>
       <c r="K139" s="17"/>
       <c r="L139" s="17"/>
       <c r="M139" s="29"/>
       <c r="N139" s="29"/>
     </row>
-    <row r="140" spans="10:14">
+    <row r="140" spans="1:14">
       <c r="J140" s="17"/>
       <c r="K140" s="17"/>
       <c r="L140" s="17"/>
       <c r="M140" s="29"/>
       <c r="N140" s="29"/>
     </row>
-    <row r="141" spans="10:12">
+    <row r="141" spans="1:14">
       <c r="J141" s="17"/>
       <c r="K141" s="17"/>
       <c r="L141" s="17"/>
     </row>
-    <row r="142" spans="10:12">
+    <row r="142" spans="1:14">
       <c r="J142" s="17"/>
       <c r="K142" s="17"/>
       <c r="L142" s="17"/>
     </row>
-    <row r="143" spans="10:12">
+    <row r="143" spans="1:14">
       <c r="J143" s="17"/>
       <c r="K143" s="17"/>
       <c r="L143" s="17"/>
     </row>
-    <row r="144" spans="10:12">
+    <row r="144" spans="1:14">
       <c r="J144" s="17"/>
       <c r="K144" s="17"/>
       <c r="L144" s="17"/>
@@ -8075,63 +7514,66 @@
       <c r="L166" s="17"/>
       <c r="M166" s="17"/>
     </row>
-    <row r="167" spans="13:13">
+    <row r="167" spans="10:13">
       <c r="M167" s="17"/>
     </row>
-    <row r="168" spans="13:13">
+    <row r="168" spans="10:13">
       <c r="M168" s="17"/>
     </row>
-    <row r="169" spans="13:13">
+    <row r="169" spans="10:13">
       <c r="M169" s="17"/>
     </row>
-    <row r="170" spans="13:13">
+    <row r="170" spans="10:13">
       <c r="M170" s="17"/>
     </row>
-    <row r="171" spans="13:13">
+    <row r="171" spans="10:13">
       <c r="M171" s="17"/>
     </row>
-    <row r="172" spans="13:13">
+    <row r="172" spans="10:13">
       <c r="M172" s="17"/>
     </row>
-    <row r="173" spans="13:13">
+    <row r="173" spans="10:13">
       <c r="M173" s="17"/>
     </row>
-    <row r="174" spans="13:13">
+    <row r="174" spans="10:13">
       <c r="M174" s="17"/>
     </row>
-    <row r="175" spans="13:13">
+    <row r="175" spans="10:13">
       <c r="M175" s="17"/>
     </row>
-    <row r="176" spans="13:13">
+    <row r="176" spans="10:13">
       <c r="M176" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:J50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="45" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
-    <col min="8" max="8" width="11.375" customWidth="1"/>
-    <col min="9" max="9" width="11.75" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="9.75" customWidth="1"/>
+    <col min="3" max="3" width="49.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.375" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="7" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="10.75" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="9.75" customWidth="1"/>
+    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>356</v>
       </c>
@@ -8159,11 +7601,14 @@
       <c r="I1" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -8192,10 +7637,13 @@
         <v>54</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -8223,11 +7671,14 @@
       <c r="I3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="31" t="s">
+        <v>449</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
         <v>2000</v>
       </c>
@@ -8258,8 +7709,11 @@
       <c r="J4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" ht="27" spans="1:10">
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="27">
       <c r="A5">
         <v>2010</v>
       </c>
@@ -8288,10 +7742,13 @@
         <v>10</v>
       </c>
       <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
         <v>2001</v>
       </c>
     </row>
-    <row r="6" ht="27" spans="1:10">
+    <row r="6" spans="1:11" ht="27">
       <c r="A6">
         <v>2110</v>
       </c>
@@ -8320,10 +7777,13 @@
         <v>8</v>
       </c>
       <c r="J6">
+        <v>8</v>
+      </c>
+      <c r="K6">
         <v>2101</v>
       </c>
     </row>
-    <row r="7" ht="27" spans="1:10">
+    <row r="7" spans="1:11" ht="27">
       <c r="A7">
         <v>2210</v>
       </c>
@@ -8352,14 +7812,17 @@
         <v>12</v>
       </c>
       <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
         <v>2201</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="1:11">
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" ht="27" spans="1:10">
+    <row r="9" spans="1:11" ht="27">
       <c r="A9" s="1">
         <v>2020</v>
       </c>
@@ -8387,11 +7850,14 @@
       <c r="I9">
         <v>10</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="32">
+        <v>30</v>
+      </c>
+      <c r="K9">
         <v>2002</v>
       </c>
     </row>
-    <row r="10" ht="27" spans="1:10">
+    <row r="10" spans="1:11" ht="27">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -8419,11 +7885,14 @@
       <c r="I10">
         <v>6</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="32">
+        <v>50</v>
+      </c>
+      <c r="K10">
         <v>2003</v>
       </c>
     </row>
-    <row r="11" ht="27" spans="1:10">
+    <row r="11" spans="1:11" ht="27">
       <c r="A11">
         <v>2022</v>
       </c>
@@ -8451,11 +7920,14 @@
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="32">
+        <v>70</v>
+      </c>
+      <c r="K11">
         <v>2004</v>
       </c>
     </row>
-    <row r="12" ht="27" spans="1:10">
+    <row r="12" spans="1:11" ht="27">
       <c r="A12">
         <v>2023</v>
       </c>
@@ -8483,11 +7955,14 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="K12">
         <v>2005</v>
       </c>
     </row>
-    <row r="13" ht="27" spans="1:10">
+    <row r="13" spans="1:11" ht="27">
       <c r="A13">
         <v>2120</v>
       </c>
@@ -8515,11 +7990,14 @@
       <c r="I13">
         <v>8</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="32">
+        <v>24</v>
+      </c>
+      <c r="K13">
         <v>2102</v>
       </c>
     </row>
-    <row r="14" ht="27" spans="1:10">
+    <row r="14" spans="1:11" ht="27">
       <c r="A14">
         <v>2121</v>
       </c>
@@ -8547,11 +8025,14 @@
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="32">
+        <v>36</v>
+      </c>
+      <c r="K14">
         <v>2103</v>
       </c>
     </row>
-    <row r="15" ht="27" spans="1:10">
+    <row r="15" spans="1:11" ht="27">
       <c r="A15">
         <v>2122</v>
       </c>
@@ -8579,11 +8060,14 @@
       <c r="I15">
         <v>20</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="32">
+        <v>48</v>
+      </c>
+      <c r="K15">
         <v>2104</v>
       </c>
     </row>
-    <row r="16" ht="27" spans="1:10">
+    <row r="16" spans="1:11" ht="27">
       <c r="A16">
         <v>2123</v>
       </c>
@@ -8611,11 +8095,14 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="32">
+        <v>20</v>
+      </c>
+      <c r="K16">
         <v>2105</v>
       </c>
     </row>
-    <row r="17" ht="27" spans="1:10">
+    <row r="17" spans="1:11" ht="27">
       <c r="A17">
         <v>2220</v>
       </c>
@@ -8643,11 +8130,14 @@
       <c r="I17">
         <v>12</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="32">
+        <v>25</v>
+      </c>
+      <c r="K17">
         <v>2202</v>
       </c>
     </row>
-    <row r="18" ht="27" spans="1:10">
+    <row r="18" spans="1:11" ht="27">
       <c r="A18">
         <v>2221</v>
       </c>
@@ -8675,11 +8165,14 @@
       <c r="I18">
         <v>8</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="32">
+        <v>36</v>
+      </c>
+      <c r="K18">
         <v>2203</v>
       </c>
     </row>
-    <row r="19" ht="40.5" spans="1:10">
+    <row r="19" spans="1:11" ht="40.5">
       <c r="A19">
         <v>2222</v>
       </c>
@@ -8707,11 +8200,14 @@
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="32">
+        <v>24</v>
+      </c>
+      <c r="K19">
         <v>2204</v>
       </c>
     </row>
-    <row r="20" ht="40.5" spans="1:10">
+    <row r="20" spans="1:11" ht="40.5">
       <c r="A20">
         <v>2223</v>
       </c>
@@ -8739,14 +8235,18 @@
       <c r="I20">
         <v>0</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="32">
+        <v>50</v>
+      </c>
+      <c r="K20">
         <v>2205</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="1:11">
       <c r="B21" s="8"/>
-    </row>
-    <row r="22" ht="27" spans="1:10">
+      <c r="J21" s="32"/>
+    </row>
+    <row r="22" spans="1:11" ht="27">
       <c r="A22" s="1">
         <v>2030</v>
       </c>
@@ -8774,11 +8274,14 @@
       <c r="I22">
         <v>10</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="32">
+        <v>100</v>
+      </c>
+      <c r="K22">
         <v>2006</v>
       </c>
     </row>
-    <row r="23" ht="27" spans="1:10">
+    <row r="23" spans="1:11" ht="27">
       <c r="A23">
         <v>2031</v>
       </c>
@@ -8806,11 +8309,14 @@
       <c r="I23">
         <v>6</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="32">
+        <v>120</v>
+      </c>
+      <c r="K23">
         <v>2007</v>
       </c>
     </row>
-    <row r="24" ht="40.5" spans="1:10">
+    <row r="24" spans="1:11" ht="40.5">
       <c r="A24">
         <v>2032</v>
       </c>
@@ -8838,11 +8344,14 @@
       <c r="I24">
         <v>0</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="32">
+        <v>0</v>
+      </c>
+      <c r="K24">
         <v>2008</v>
       </c>
     </row>
-    <row r="25" ht="40.5" spans="1:10">
+    <row r="25" spans="1:11" ht="40.5">
       <c r="A25" s="10">
         <v>2033</v>
       </c>
@@ -8870,11 +8379,14 @@
       <c r="I25" s="10">
         <v>10</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="32">
+        <v>200</v>
+      </c>
+      <c r="K25" s="10">
         <v>2009</v>
       </c>
     </row>
-    <row r="26" ht="40.5" spans="1:10">
+    <row r="26" spans="1:11" ht="40.5">
       <c r="A26" s="10">
         <v>2034</v>
       </c>
@@ -8902,11 +8414,14 @@
       <c r="I26" s="10">
         <v>0</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="32">
+        <v>0.15</v>
+      </c>
+      <c r="K26" s="10">
         <v>2010</v>
       </c>
     </row>
-    <row r="27" ht="27" spans="1:10">
+    <row r="27" spans="1:11" ht="27">
       <c r="A27" s="10">
         <v>2130</v>
       </c>
@@ -8934,11 +8449,14 @@
       <c r="I27" s="10">
         <v>8</v>
       </c>
-      <c r="J27" s="10">
+      <c r="J27" s="32">
+        <v>120</v>
+      </c>
+      <c r="K27" s="10">
         <v>2106</v>
       </c>
     </row>
-    <row r="28" ht="27" spans="1:10">
+    <row r="28" spans="1:11" ht="27">
       <c r="A28" s="10">
         <v>2131</v>
       </c>
@@ -8966,11 +8484,14 @@
       <c r="I28" s="10">
         <v>15</v>
       </c>
-      <c r="J28" s="10">
+      <c r="J28" s="32">
+        <v>80</v>
+      </c>
+      <c r="K28" s="10">
         <v>2107</v>
       </c>
     </row>
-    <row r="29" ht="40.5" spans="1:10">
+    <row r="29" spans="1:11" ht="40.5">
       <c r="A29" s="10">
         <v>2132</v>
       </c>
@@ -8998,11 +8519,14 @@
       <c r="I29" s="10">
         <v>0</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29" s="32">
+        <v>0.12</v>
+      </c>
+      <c r="K29" s="10">
         <v>2108</v>
       </c>
     </row>
-    <row r="30" ht="40.5" spans="1:10">
+    <row r="30" spans="1:11" ht="40.5">
       <c r="A30" s="10">
         <v>2133</v>
       </c>
@@ -9030,11 +8554,14 @@
       <c r="I30" s="10">
         <v>0</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J30" s="32">
+        <v>88</v>
+      </c>
+      <c r="K30" s="10">
         <v>2109</v>
       </c>
     </row>
-    <row r="31" ht="40.5" spans="1:10">
+    <row r="31" spans="1:11" ht="40.5">
       <c r="A31" s="10">
         <v>2134</v>
       </c>
@@ -9062,11 +8589,14 @@
       <c r="I31" s="10">
         <v>180</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J31" s="32">
+        <v>66</v>
+      </c>
+      <c r="K31" s="10">
         <v>2110</v>
       </c>
     </row>
-    <row r="32" ht="27" spans="1:10">
+    <row r="32" spans="1:11" ht="27">
       <c r="A32" s="10">
         <v>2230</v>
       </c>
@@ -9094,11 +8624,14 @@
       <c r="I32" s="10">
         <v>12</v>
       </c>
-      <c r="J32" s="10">
+      <c r="J32" s="32">
+        <v>120</v>
+      </c>
+      <c r="K32" s="10">
         <v>2206</v>
       </c>
     </row>
-    <row r="33" ht="27" spans="1:10">
+    <row r="33" spans="1:11" ht="27">
       <c r="A33" s="10">
         <v>2231</v>
       </c>
@@ -9126,11 +8659,14 @@
       <c r="I33" s="10">
         <v>19</v>
       </c>
-      <c r="J33" s="10">
+      <c r="J33" s="32">
+        <v>90</v>
+      </c>
+      <c r="K33" s="10">
         <v>2207</v>
       </c>
     </row>
-    <row r="34" ht="40.5" spans="1:10">
+    <row r="34" spans="1:11" ht="40.5">
       <c r="A34" s="10">
         <v>2232</v>
       </c>
@@ -9158,11 +8694,14 @@
       <c r="I34" s="10">
         <v>0</v>
       </c>
-      <c r="J34" s="10">
+      <c r="J34" s="32">
+        <v>0.12</v>
+      </c>
+      <c r="K34" s="10">
         <v>2208</v>
       </c>
     </row>
-    <row r="35" ht="27" spans="1:10">
+    <row r="35" spans="1:11" ht="27">
       <c r="A35" s="10">
         <v>2233</v>
       </c>
@@ -9190,11 +8729,14 @@
       <c r="I35" s="10">
         <v>12</v>
       </c>
-      <c r="J35" s="10">
+      <c r="J35" s="32">
+        <v>150</v>
+      </c>
+      <c r="K35" s="10">
         <v>2209</v>
       </c>
     </row>
-    <row r="36" ht="40.5" spans="1:10">
+    <row r="36" spans="1:11" ht="40.5">
       <c r="A36" s="10">
         <v>2234</v>
       </c>
@@ -9222,11 +8764,14 @@
       <c r="I36" s="10">
         <v>0</v>
       </c>
-      <c r="J36" s="10">
+      <c r="J36" s="32">
+        <v>0</v>
+      </c>
+      <c r="K36" s="10">
         <v>2210</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:11">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="13"/>
@@ -9236,9 +8781,10 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-    </row>
-    <row r="38" ht="27" spans="1:10">
+      <c r="J37" s="32"/>
+      <c r="K37" s="10"/>
+    </row>
+    <row r="38" spans="1:11" ht="27">
       <c r="A38" s="10">
         <v>2040</v>
       </c>
@@ -9266,11 +8812,14 @@
       <c r="I38" s="10">
         <v>20</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J38" s="32">
+        <v>150</v>
+      </c>
+      <c r="K38" s="10">
         <v>2011</v>
       </c>
     </row>
-    <row r="39" ht="31.5" spans="1:10">
+    <row r="39" spans="1:11" ht="31.5">
       <c r="A39" s="10">
         <v>2041</v>
       </c>
@@ -9298,11 +8847,14 @@
       <c r="I39" s="10">
         <v>10</v>
       </c>
-      <c r="J39" s="10">
+      <c r="J39" s="32">
+        <v>180</v>
+      </c>
+      <c r="K39" s="10">
         <v>2012</v>
       </c>
     </row>
-    <row r="40" ht="40.5" spans="1:10">
+    <row r="40" spans="1:11" ht="40.5">
       <c r="A40" s="10">
         <v>2042</v>
       </c>
@@ -9330,11 +8882,14 @@
       <c r="I40" s="10">
         <v>0</v>
       </c>
-      <c r="J40" s="10">
+      <c r="J40" s="32">
+        <v>0</v>
+      </c>
+      <c r="K40" s="10">
         <v>2013</v>
       </c>
     </row>
-    <row r="41" ht="40.5" spans="1:10">
+    <row r="41" spans="1:11" ht="40.5">
       <c r="A41" s="10">
         <v>2140</v>
       </c>
@@ -9362,11 +8917,14 @@
       <c r="I41" s="10">
         <v>15</v>
       </c>
-      <c r="J41" s="10">
+      <c r="J41" s="32">
+        <v>125</v>
+      </c>
+      <c r="K41" s="10">
         <v>2111</v>
       </c>
     </row>
-    <row r="42" ht="27" spans="1:10">
+    <row r="42" spans="1:11" ht="27">
       <c r="A42" s="10">
         <v>2141</v>
       </c>
@@ -9394,11 +8952,14 @@
       <c r="I42" s="15">
         <v>0</v>
       </c>
-      <c r="J42" s="10">
+      <c r="J42" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="K42" s="10">
         <v>2112</v>
       </c>
     </row>
-    <row r="43" ht="27" spans="1:10">
+    <row r="43" spans="1:11" ht="27">
       <c r="A43" s="10">
         <v>2240</v>
       </c>
@@ -9426,11 +8987,14 @@
       <c r="I43" s="10">
         <v>38</v>
       </c>
-      <c r="J43" s="10">
+      <c r="J43" s="32">
+        <v>133</v>
+      </c>
+      <c r="K43" s="10">
         <v>2211</v>
       </c>
     </row>
-    <row r="44" ht="27" spans="1:10">
+    <row r="44" spans="1:11" ht="27">
       <c r="A44" s="10">
         <v>2241</v>
       </c>
@@ -9458,11 +9022,14 @@
       <c r="I44" s="15">
         <v>0</v>
       </c>
-      <c r="J44" s="10">
+      <c r="J44" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="K44" s="10">
         <v>2212</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:11">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="13"/>
@@ -9473,8 +9040,9 @@
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45" s="10"/>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>4001</v>
       </c>
@@ -9502,11 +9070,11 @@
       <c r="I46">
         <v>0</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>4001</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>4005</v>
       </c>
@@ -9514,11 +9082,12 @@
         <v>441</v>
       </c>
       <c r="I47" s="17"/>
-      <c r="J47">
+      <c r="J47" s="17"/>
+      <c r="K47">
         <v>4005</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>4006</v>
       </c>
@@ -9526,11 +9095,12 @@
         <v>442</v>
       </c>
       <c r="I48" s="17"/>
-      <c r="J48">
+      <c r="J48" s="17"/>
+      <c r="K48">
         <v>4006</v>
       </c>
     </row>
-    <row r="49" ht="14.25" spans="1:10">
+    <row r="49" spans="1:11" ht="14.25">
       <c r="A49">
         <v>4007</v>
       </c>
@@ -9541,11 +9111,12 @@
         <v>444</v>
       </c>
       <c r="I49" s="17"/>
-      <c r="J49">
+      <c r="J49" s="17"/>
+      <c r="K49">
         <v>4007</v>
       </c>
     </row>
-    <row r="50" ht="14.25" spans="1:10">
+    <row r="50" spans="1:11" ht="14.25">
       <c r="A50">
         <v>4008</v>
       </c>
@@ -9555,13 +9126,13 @@
       <c r="C50" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>4008</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Balance the cost and recovery of magic.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/ItemData.xlsx
+++ b/Documents/ExcelData/ItemData.xlsx
@@ -2301,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q176"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7555,8 +7555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7742,7 +7742,7 @@
         <v>10</v>
       </c>
       <c r="J5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K5">
         <v>2001</v>
@@ -7777,7 +7777,7 @@
         <v>8</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K6">
         <v>2101</v>
@@ -7812,7 +7812,7 @@
         <v>12</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K7">
         <v>2201</v>
@@ -7851,7 +7851,7 @@
         <v>10</v>
       </c>
       <c r="J9" s="32">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K9">
         <v>2002</v>
@@ -7886,7 +7886,7 @@
         <v>6</v>
       </c>
       <c r="J10" s="32">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="K10">
         <v>2003</v>
@@ -7921,7 +7921,7 @@
         <v>10</v>
       </c>
       <c r="J11" s="32">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="K11">
         <v>2004</v>
@@ -7991,7 +7991,7 @@
         <v>8</v>
       </c>
       <c r="J13" s="32">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K13">
         <v>2102</v>
@@ -8026,7 +8026,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="32">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="K14">
         <v>2103</v>
@@ -8061,7 +8061,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="32">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="K15">
         <v>2104</v>
@@ -8131,7 +8131,7 @@
         <v>12</v>
       </c>
       <c r="J17" s="32">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="K17">
         <v>2202</v>
@@ -8166,7 +8166,7 @@
         <v>8</v>
       </c>
       <c r="J18" s="32">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K18">
         <v>2203</v>
@@ -8275,7 +8275,7 @@
         <v>10</v>
       </c>
       <c r="J22" s="32">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="K22">
         <v>2006</v>
@@ -8310,7 +8310,7 @@
         <v>6</v>
       </c>
       <c r="J23" s="32">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="K23">
         <v>2007</v>
@@ -8351,7 +8351,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="40.5">
+    <row r="25" spans="1:11" ht="27">
       <c r="A25" s="10">
         <v>2033</v>
       </c>
@@ -8450,7 +8450,7 @@
         <v>8</v>
       </c>
       <c r="J27" s="32">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="K27" s="10">
         <v>2106</v>
@@ -8526,7 +8526,7 @@
         <v>2108</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="40.5">
+    <row r="30" spans="1:11" ht="27">
       <c r="A30" s="10">
         <v>2133</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="32">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="K30" s="10">
         <v>2109</v>
@@ -8590,7 +8590,7 @@
         <v>180</v>
       </c>
       <c r="J31" s="32">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="K31" s="10">
         <v>2110</v>
@@ -8625,7 +8625,7 @@
         <v>12</v>
       </c>
       <c r="J32" s="32">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="K32" s="10">
         <v>2206</v>
@@ -8660,7 +8660,7 @@
         <v>19</v>
       </c>
       <c r="J33" s="32">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="K33" s="10">
         <v>2207</v>
@@ -8730,7 +8730,7 @@
         <v>12</v>
       </c>
       <c r="J35" s="32">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="K35" s="10">
         <v>2209</v>
@@ -8819,7 +8819,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="31.5">
+    <row r="39" spans="1:11" ht="30">
       <c r="A39" s="10">
         <v>2041</v>
       </c>
@@ -8889,7 +8889,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="40.5">
+    <row r="41" spans="1:11" ht="27">
       <c r="A41" s="10">
         <v>2140</v>
       </c>
@@ -9053,10 +9053,10 @@
         <v>440</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E46">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="F46">
         <v>100</v>
@@ -9069,6 +9069,9 @@
       </c>
       <c r="I46">
         <v>0</v>
+      </c>
+      <c r="J46" s="10">
+        <v>5</v>
       </c>
       <c r="K46">
         <v>4001</v>

</xml_diff>

<commit_message>
Add switch attack for all of short swords.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/ItemData.xlsx
+++ b/Documents/ExcelData/ItemData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="463">
   <si>
     <t>物品ID</t>
   </si>
@@ -1621,6 +1621,197 @@
   </si>
   <si>
     <t>势大力沉的重型弩炮。在与野兽的战斗中很少有人使用远程武器，因为一旦被敌人接近将造成不可挽回的后果。但这种弩的发明，使得人们可以在远处就可以较为安全地将兽们轰杀至渣。</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>100,1</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00</t>
+    </r>
     <phoneticPr fontId="14" type="noConversion"/>
   </si>
 </sst>
@@ -1772,7 +1963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1861,6 +2052,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2354,8 +2548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="K93" sqref="K93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2639,11 +2833,11 @@
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
       <c r="O5" s="24"/>
-      <c r="P5" s="24">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="24">
-        <v>1</v>
+      <c r="P5" s="24" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>454</v>
       </c>
       <c r="R5" s="24"/>
       <c r="S5" s="35">
@@ -2699,11 +2893,11 @@
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
       <c r="O6" s="24"/>
-      <c r="P6" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q6" s="24" t="s">
-        <v>74</v>
+      <c r="P6" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q6" s="37" t="s">
+        <v>456</v>
       </c>
       <c r="R6" s="24"/>
       <c r="S6" s="35">
@@ -2759,11 +2953,11 @@
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
       <c r="O7" s="24"/>
-      <c r="P7" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q7" s="24" t="s">
-        <v>73</v>
+      <c r="P7" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q7" s="37" t="s">
+        <v>457</v>
       </c>
       <c r="R7" s="24"/>
       <c r="S7" s="35">
@@ -2819,11 +3013,11 @@
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
       <c r="O8" s="24"/>
-      <c r="P8" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q8" s="24" t="s">
-        <v>85</v>
+      <c r="P8" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q8" s="37" t="s">
+        <v>458</v>
       </c>
       <c r="R8" s="24"/>
       <c r="S8" s="35">
@@ -2879,11 +3073,11 @@
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
       <c r="O9" s="24"/>
-      <c r="P9" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q9" s="24" t="s">
-        <v>91</v>
+      <c r="P9" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q9" s="37" t="s">
+        <v>459</v>
       </c>
       <c r="R9" s="24"/>
       <c r="S9" s="35">
@@ -2939,11 +3133,11 @@
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
       <c r="O10" s="24"/>
-      <c r="P10" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q10" s="24" t="s">
-        <v>96</v>
+      <c r="P10" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q10" s="37" t="s">
+        <v>460</v>
       </c>
       <c r="R10" s="24"/>
       <c r="S10" s="35">
@@ -3031,8 +3225,12 @@
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
       <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
+      <c r="P12" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q12" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R12" s="24"/>
       <c r="S12" s="35">
         <f t="shared" si="0"/>
@@ -3087,8 +3285,12 @@
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
       <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
+      <c r="P13" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q13" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R13" s="24"/>
       <c r="S13" s="35">
         <f t="shared" si="0"/>
@@ -3143,8 +3345,12 @@
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
       <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
+      <c r="P14" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q14" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R14" s="24"/>
       <c r="S14" s="35">
         <f t="shared" si="0"/>
@@ -3199,8 +3405,12 @@
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
       <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
+      <c r="P15" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q15" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R15" s="24"/>
       <c r="S15" s="35">
         <f t="shared" si="0"/>
@@ -3255,8 +3465,12 @@
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
       <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
+      <c r="P16" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q16" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R16" s="24"/>
       <c r="S16" s="35">
         <f t="shared" si="0"/>
@@ -3311,8 +3525,12 @@
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
       <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
+      <c r="P17" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q17" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R17" s="24"/>
       <c r="S17" s="35">
         <f t="shared" si="0"/>
@@ -3399,8 +3617,12 @@
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
       <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
+      <c r="P19" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q19" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R19" s="24"/>
       <c r="S19" s="35">
         <f t="shared" si="0"/>
@@ -3455,8 +3677,12 @@
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
       <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
+      <c r="P20" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q20" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R20" s="24"/>
       <c r="S20" s="35">
         <f t="shared" si="0"/>
@@ -3511,8 +3737,12 @@
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
       <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
+      <c r="P21" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q21" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R21" s="24"/>
       <c r="S21" s="35">
         <f t="shared" si="0"/>
@@ -3567,8 +3797,12 @@
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
       <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
+      <c r="P22" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q22" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R22" s="24"/>
       <c r="S22" s="35">
         <f t="shared" si="0"/>
@@ -3623,8 +3857,12 @@
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
       <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
+      <c r="P23" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q23" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R23" s="24"/>
       <c r="S23" s="35">
         <f t="shared" si="0"/>
@@ -3679,8 +3917,12 @@
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
       <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
+      <c r="P24" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q24" s="37" t="s">
+        <v>462</v>
+      </c>
       <c r="R24" s="24"/>
       <c r="S24" s="35">
         <f t="shared" si="0"/>
@@ -9056,7 +9298,7 @@
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>